<commit_message>
updated status_key.xslx and status.py
status_key.xlsx: removed “Unavailable”
status.py: fixed bug in printing uframe_route column
</commit_message>
<xml_diff>
--- a/tools/ingestion_status/Satus_key.xlsx
+++ b/tools/ingestion_status/Satus_key.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38860" yWindow="11480" windowWidth="21480" windowHeight="10180" tabRatio="500"/>
+    <workbookView xWindow="13880" yWindow="5480" windowWidth="23980" windowHeight="10360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>Not Deployed</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Available</t>
   </si>
   <si>
-    <t>Unavailable</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
@@ -67,12 +64,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>Data not to be delivered — Not telemetered, Not recorded, or Lost in transmission</t>
   </si>
   <si>
     <t>Data Delivery Status</t>
@@ -196,6 +187,9 @@
   </si>
   <si>
     <t>Not Expected</t>
+  </si>
+  <si>
+    <t>Data not to be delivered — Not telemetered, Not recorded, Lost in transmission, Instrument failed/damaged</t>
   </si>
 </sst>
 </file>
@@ -279,7 +273,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,12 +343,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF44DCE6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE636D8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,7 +369,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -409,9 +397,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -707,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,26 +703,26 @@
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -746,10 +731,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" t="s">
@@ -762,14 +747,14 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="19"/>
+        <v>6</v>
+      </c>
+      <c r="E3" s="3"/>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -781,11 +766,11 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="E4" s="4"/>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -797,11 +782,11 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="E5" s="18"/>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -813,11 +798,11 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -829,31 +814,18 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
+      <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
@@ -887,9 +859,6 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -914,7 +883,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
@@ -923,154 +892,154 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
       <c r="F2" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
       <c r="B3" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="15"/>
       <c r="B8" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>